<commit_message>
Added Glove pre-trained legal embeddings
</commit_message>
<xml_diff>
--- a/modeling/results/final_results_acc.xlsx
+++ b/modeling/results/final_results_acc.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Features</t>
   </si>
@@ -31,6 +31,9 @@
     <t>SVM</t>
   </si>
   <si>
+    <t>baseline</t>
+  </si>
+  <si>
     <t>N-Grams + Attr</t>
   </si>
   <si>
@@ -38,6 +41,12 @@
   </si>
   <si>
     <t>N-Grams</t>
+  </si>
+  <si>
+    <t>Embeddings</t>
+  </si>
+  <si>
+    <t>Embeddings + Attr</t>
   </si>
 </sst>
 </file>
@@ -395,13 +404,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -417,56 +426,108 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2">
-        <v>0.8120000000000001</v>
+        <v>0.797</v>
       </c>
       <c r="C2">
-        <v>0.643</v>
+        <v>0.792</v>
       </c>
       <c r="D2">
-        <v>0.8100000000000001</v>
+        <v>0.797</v>
       </c>
       <c r="E2">
-        <v>0.82</v>
+        <v>0.797</v>
+      </c>
+      <c r="F2">
+        <v>0.756</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>0.744</v>
+        <v>0.748</v>
       </c>
       <c r="C3">
-        <v>0.594</v>
+        <v>0.27</v>
       </c>
       <c r="D3">
-        <v>0.732</v>
+        <v>0.74</v>
       </c>
       <c r="E3">
-        <v>0.74</v>
+        <v>0.738</v>
+      </c>
+      <c r="F3">
+        <v>0.743</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>0.789</v>
+        <v>0.782</v>
       </c>
       <c r="C4">
-        <v>0.594</v>
+        <v>0.782</v>
       </c>
       <c r="D4">
-        <v>0.782</v>
+        <v>0.771</v>
       </c>
       <c r="E4">
+        <v>0.795</v>
+      </c>
+      <c r="F4">
+        <v>0.743</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>0.801</v>
+      </c>
+      <c r="C5">
+        <v>0.63</v>
+      </c>
+      <c r="D5">
+        <v>0.778</v>
+      </c>
+      <c r="E5">
         <v>0.786</v>
+      </c>
+      <c r="F5">
+        <v>0.742</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>0.755</v>
+      </c>
+      <c r="C6">
+        <v>0.269</v>
+      </c>
+      <c r="D6">
+        <v>0.755</v>
+      </c>
+      <c r="E6">
+        <v>0.775</v>
+      </c>
+      <c r="F6">
+        <v>0.747</v>
       </c>
     </row>
   </sheetData>

</xml_diff>